<commit_message>
Se ha continuado con el desarrollo del CU3 y se ha iniciado y concluido el CU7 Ingresar a sitio web, se agregó el mensaje MSG7, MSG8 y MSG9, se ha creado una presentación del algoritmo propuesto para recolectar las noticias, se cálcula  el mejor camino para recolectar la información, con base en el número de vistas de la página
</commit_message>
<xml_diff>
--- a/Seguimiento/CronogramaPorMes.xlsx
+++ b/Seguimiento/CronogramaPorMes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Andrew/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Andrew/Documents/TT1/TT1/Seguimiento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5843ABF3-7D6B-BB49-8655-841A599A7742}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33F8E7F-22BC-3D41-918A-1FD705A7271B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actividades Andres" sheetId="3" r:id="rId1"/>
@@ -351,10 +351,10 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -678,7 +678,7 @@
   <dimension ref="A2:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -887,10 +887,10 @@
       <c r="J14" s="7"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="25"/>
+      <c r="B16" s="26"/>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1">
       <c r="A17" s="8" t="s">
@@ -960,7 +960,9 @@
   </sheetPr>
   <dimension ref="B2:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -1161,7 +1163,7 @@
       <c r="B15" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="25"/>
+      <c r="C15" s="26"/>
     </row>
     <row r="16" spans="2:11" ht="15.75" customHeight="1">
       <c r="B16" s="20" t="s">

</xml_diff>